<commit_message>
change template in french
</commit_message>
<xml_diff>
--- a/input/Template_Population_figures.xlsx
+++ b/input/Template_Population_figures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/pin-calculation-app/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="8_{D63770E9-8D5C-4F2A-BD7D-98D3C6683B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FC0DE84-82BC-417C-A302-2F24B82D41ED}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="8_{D63770E9-8D5C-4F2A-BD7D-98D3C6683B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B669CEC-EDF6-47CD-A1B1-466A4DC62FC2}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{24D09A16-471A-4A7F-BD10-C475AB78837D}"/>
   </bookViews>
@@ -102,49 +102,49 @@
     <t>Admin Pcode</t>
   </si>
   <si>
-    <t>Children (5-17)</t>
-  </si>
-  <si>
-    <t>Girls  (5-17)</t>
-  </si>
-  <si>
-    <t>Boys  (5-17)</t>
-  </si>
-  <si>
-    <t>Host -- Children (5-17)</t>
-  </si>
-  <si>
-    <t>Host -- Girls  (5-17)</t>
-  </si>
-  <si>
-    <t>Host -- Boys  (5-17)</t>
-  </si>
-  <si>
-    <t>IDP -- Children (5-17)</t>
-  </si>
-  <si>
-    <t>IDP -- Girls  (5-17)</t>
-  </si>
-  <si>
-    <t>IDP -- Boys  (5-17)</t>
-  </si>
-  <si>
-    <t>Returnees -- Children (5-17)</t>
-  </si>
-  <si>
-    <t>Returnees -- Girls  (5-17)</t>
-  </si>
-  <si>
-    <t>Returnees -- Boys  (5-17)</t>
-  </si>
-  <si>
-    <t>Refugees -- Children (5-17)</t>
-  </si>
-  <si>
-    <t>Refugees -- Girls  (5-17)</t>
-  </si>
-  <si>
-    <t>Refugees -- Boys  (5-17)</t>
+    <t>IDP/PDI -- Children (5-17)</t>
+  </si>
+  <si>
+    <t>Refugees/Refugiee -- Children (5-17)</t>
+  </si>
+  <si>
+    <t>Refugees/Refugiee -- Girls  (5-17)</t>
+  </si>
+  <si>
+    <t>Refugees/Refugiee -- Boys  (5-17)</t>
+  </si>
+  <si>
+    <t>Returnees/Retournés -- Children (5-17)</t>
+  </si>
+  <si>
+    <t>Returnees/Retournés -- Girls  (5-17)</t>
+  </si>
+  <si>
+    <t>Returnees/Retournés -- Boys  (5-17)</t>
+  </si>
+  <si>
+    <t>IDP/PDI -- Girls  (5-17)</t>
+  </si>
+  <si>
+    <t>IDP/PDI -- Boys  (5-17)</t>
+  </si>
+  <si>
+    <t>Host/Hôte-- Children (5-17)</t>
+  </si>
+  <si>
+    <t>Host/Hôte -- Girls  (5-17)</t>
+  </si>
+  <si>
+    <t>Host/Hôte -- Boys  (5-17)</t>
+  </si>
+  <si>
+    <t>Children/Enfants (5-17)</t>
+  </si>
+  <si>
+    <t>Girls/Filles  (5-17)</t>
+  </si>
+  <si>
+    <t>Boys/Garcons  (5-17)</t>
   </si>
 </sst>
 </file>
@@ -700,7 +700,7 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -733,25 +733,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>8</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>9</v>
@@ -760,22 +760,22 @@
         <v>10</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="Q1" s="13" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="R1" s="14"/>
       <c r="S1" s="14"/>

</xml_diff>

<commit_message>
adding a important check on the upoloaded population data
</commit_message>
<xml_diff>
--- a/input/Template_Population_figures.xlsx
+++ b/input/Template_Population_figures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/pin-calculation-app/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="8_{D63770E9-8D5C-4F2A-BD7D-98D3C6683B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C4C6140-CC68-4C67-84BA-ED7177D87566}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="8_{D63770E9-8D5C-4F2A-BD7D-98D3C6683B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8AE61E7-15E9-4966-B0BD-7B98F80E24B0}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{24D09A16-471A-4A7F-BD10-C475AB78837D}"/>
+    <workbookView xWindow="13380" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{24D09A16-471A-4A7F-BD10-C475AB78837D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Admin</t>
   </si>
@@ -108,24 +108,6 @@
     <t>Returnees/Retournés -- Children/Enfants (5-17)</t>
   </si>
   <si>
-    <t>Host/Hôte -- Girls/Filles (5-17)</t>
-  </si>
-  <si>
-    <t>Host/Hôte -- Boys/Garcons (5-17)</t>
-  </si>
-  <si>
-    <t>IDP/PDI -- Girls/Filles (5-17)</t>
-  </si>
-  <si>
-    <t>IDP/PDI -- Boys/Garcons (5-17)</t>
-  </si>
-  <si>
-    <t>Returnees/Retournés -- Girls/Filles (5-17)</t>
-  </si>
-  <si>
-    <t>Returnees/Retournés -- Boys/Garcons (5-17)</t>
-  </si>
-  <si>
     <t>Host/Hôte -- Children/Enfants (5-17)</t>
   </si>
   <si>
@@ -141,29 +123,23 @@
     <t>Refugees/Refugiees -- Children/Enfants (5-17)</t>
   </si>
   <si>
-    <t>Refugees/Refugiees -- Girls/Filles (5-17)</t>
-  </si>
-  <si>
-    <t>Refugees/Refugiees -- Boys/Garcons (5-17)</t>
-  </si>
-  <si>
     <t>5yo -- Girls/Filles</t>
   </si>
   <si>
     <t>5yo -- Boys/Garcons</t>
   </si>
   <si>
-    <t xml:space="preserve">5yo -- Children/Enfants  </t>
-  </si>
-  <si>
     <t>Other -- Children/Enfants (5-17)</t>
+  </si>
+  <si>
+    <t>5yo -- Children/Enfants</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,13 +167,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -220,33 +189,24 @@
     <font>
       <b/>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,12 +222,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.89999084444715716"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,7 +262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -331,57 +285,25 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -390,29 +312,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -755,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA56C02-61B5-41C1-B66B-44B5B6878CC3}">
-  <dimension ref="A1:W31"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -768,81 +680,53 @@
     <col min="3" max="6" width="11.26953125" style="3" customWidth="1"/>
     <col min="7" max="8" width="9.1796875" style="5" customWidth="1"/>
     <col min="9" max="9" width="17.453125" style="3"/>
-    <col min="10" max="11" width="9.76953125" style="15" customWidth="1"/>
-    <col min="13" max="14" width="9.86328125" style="15" customWidth="1"/>
-    <col min="15" max="15" width="17.453125" style="1"/>
-    <col min="16" max="17" width="9.54296875" style="15" customWidth="1"/>
-    <col min="19" max="20" width="10.04296875" style="15" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="12" customFormat="1" ht="39.35" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:15" s="10" customFormat="1" ht="39.4" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A2" s="2"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
@@ -852,19 +736,11 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
+      <c r="J2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="17"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="1"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
@@ -874,19 +750,11 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
+      <c r="J3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="17"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="1"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
@@ -896,19 +764,11 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
+      <c r="J4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="17"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="1"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
@@ -918,19 +778,11 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
+      <c r="J5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="17"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="1"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
@@ -940,19 +792,11 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
+      <c r="J6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="17"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="1"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
@@ -962,19 +806,11 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="J7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="17"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="1"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
@@ -984,19 +820,11 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
+      <c r="J8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="17"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="1"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
@@ -1006,19 +834,11 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="J9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="17"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="1"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A10" s="2"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
@@ -1028,19 +848,11 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
+      <c r="J10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="17"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="1"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A11" s="2"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
@@ -1050,19 +862,11 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="J11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="17"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="1"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
@@ -1072,19 +876,11 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
+      <c r="J12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="17"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="1"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A13" s="2"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -1094,19 +890,11 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="J13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="17"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="1"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A14" s="2"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -1116,19 +904,11 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
+      <c r="J14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="17"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="1"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A15" s="2"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -1138,19 +918,11 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="J15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="17"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="1"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.75">
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A16" s="2"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
@@ -1160,19 +932,11 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
+      <c r="J16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="17"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="1"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A17" s="2"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
@@ -1182,19 +946,11 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
+      <c r="J17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="17"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="1"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A18" s="2"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
@@ -1204,19 +960,11 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
+      <c r="J18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="17"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="1"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A19" s="2"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
@@ -1226,19 +974,11 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
+      <c r="J19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="17"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="1"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A20" s="2"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
@@ -1248,19 +988,11 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
+      <c r="J20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="17"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="1"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A21" s="2"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
@@ -1270,19 +1002,11 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
+      <c r="J21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="17"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="1"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A22" s="2"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
@@ -1292,19 +1016,11 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
+      <c r="J22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="17"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="1"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A23" s="2"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
@@ -1314,19 +1030,11 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
+      <c r="J23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="17"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="1"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A24" s="2"/>
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
@@ -1336,19 +1044,11 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
+      <c r="J24" s="1"/>
       <c r="L24" s="1"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="17"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="1"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A25" s="2"/>
       <c r="B25" s="1"/>
       <c r="C25" s="2"/>
@@ -1358,19 +1058,11 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
+      <c r="J25" s="1"/>
       <c r="L25" s="1"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="17"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="1"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A26" s="2"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2"/>
@@ -1380,19 +1072,11 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
+      <c r="J26" s="1"/>
       <c r="L26" s="1"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="17"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="1"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A27" s="2"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
@@ -1402,19 +1086,11 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
+      <c r="J27" s="1"/>
       <c r="L27" s="1"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="17"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="1"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A28" s="2"/>
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
@@ -1424,19 +1100,11 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
+      <c r="J28" s="1"/>
       <c r="L28" s="1"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="17"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="14"/>
-      <c r="T28" s="14"/>
-      <c r="U28" s="1"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A29" s="2"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
@@ -1446,19 +1114,11 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
+      <c r="J29" s="1"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="17"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="14"/>
-      <c r="T29" s="14"/>
-      <c r="U29" s="1"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A30" s="2"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
@@ -1468,19 +1128,11 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
+      <c r="J30" s="1"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="17"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="14"/>
-      <c r="T30" s="14"/>
-      <c r="U30" s="1"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.75">
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A31" s="2"/>
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
@@ -1490,21 +1142,13 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
+      <c r="J31" s="1"/>
       <c r="L31" s="1"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="17"/>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="14"/>
-      <c r="T31" s="14"/>
-      <c r="U31" s="1"/>
+      <c r="M31" s="1"/>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="A2:U121" name="pop value"/>
+    <protectedRange sqref="A2:M121" name="pop value"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
adding check on ocha mandatory column plus flag for scope fix sheet
if it has value scope_fix == true
</commit_message>
<xml_diff>
--- a/input/Template_Population_figures.xlsx
+++ b/input/Template_Population_figures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/pin-calculation-app/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/PiN_app_dev/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="421" documentId="8_{D63770E9-8D5C-4F2A-BD7D-98D3C6683B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EA4ACF5-4497-4B57-9D46-B6A9D7AC3532}"/>
+  <xr:revisionPtr revIDLastSave="425" documentId="8_{D63770E9-8D5C-4F2A-BD7D-98D3C6683B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFE5EF5D-68D5-4EC5-941D-CB6A89F582AD}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" activeTab="1" xr2:uid="{24D09A16-471A-4A7F-BD10-C475AB78837D}"/>
+    <workbookView xWindow="-19290" yWindow="-3720" windowWidth="19380" windowHeight="11460" activeTab="1" xr2:uid="{24D09A16-471A-4A7F-BD10-C475AB78837D}"/>
   </bookViews>
   <sheets>
     <sheet name="ocha" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ocha!$A$1:$M$141</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -348,7 +348,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,6 +460,21 @@
     <font>
       <i/>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -516,12 +531,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -544,12 +558,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -583,9 +613,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 4" xfId="1" xr:uid="{71695770-2CA8-438C-96D1-ED3328163623}"/>
   </cellStyles>
@@ -991,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39D4D79-A7A6-48C8-8509-FD3F2A049ECB}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1016,22 +1048,31 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A2" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A3" s="13" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>